<commit_message>
add noxubee discharge states
</commit_message>
<xml_diff>
--- a/_analysis/dst/board-scenarios.xlsx
+++ b/_analysis/dst/board-scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcolvin\Documents\projects\Bluff-Lake-Project\analysis\dst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcolvin\Documents\projects\Bluff-Lake-Project\_analysis\dst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{497BEA0D-9E58-4FA1-A123-5EF080817B55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843FF943-6234-40E4-B2EC-D56AE76BE6D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9816" windowHeight="2676" xr2:uid="{DCE9A652-60D8-41C0-A8E8-7A64510DEF21}"/>
+    <workbookView minimized="1" xWindow="23388" yWindow="2052" windowWidth="12096" windowHeight="6936" xr2:uid="{DCE9A652-60D8-41C0-A8E8-7A64510DEF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -429,7 +430,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>